<commit_message>
feat(reporting): finalize exports + tri-state UI
- Complete XLSX/CSV builders for Aggregated/Disaggregated/Barangay; mirror UI visibility & totals
- CreateReportModal: tri-state checkboxes, age ranges; single active report type
- Cleanup TS: remove unused enabled param and reportTypes prop usage
- Templates/layout: freeze panes, widths/wraps; wrap Relief Services text
</commit_message>
<xml_diff>
--- a/server/templates/Barangay.xlsx
+++ b/server/templates/Barangay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_VicenteBercasioII\Documents\Github Projects\e-LegTas\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705020BF-1737-4206-9F7F-687D8F8CBEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7685BCF-94C8-45EE-BB27-0EE1CAF470C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72FF522A-0EE4-40AE-8972-20260110F40D}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{72FF522A-0EE4-40AE-8972-20260110F40D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Republic of the Philippines</t>
   </si>
@@ -42,91 +42,22 @@
     <t>City Government of Legazpi</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Total No. of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Male</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total No. of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Female</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total No. of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Individuals</t>
-    </r>
-  </si>
-  <si>
     <t>Infant</t>
-  </si>
-  <si>
-    <t>(1 year old)</t>
   </si>
   <si>
     <t>Children</t>
   </si>
   <si>
-    <t>(2-12 yrs. old)</t>
-  </si>
-  <si>
     <t>Youth</t>
-  </si>
-  <si>
-    <t>(13-17 yrs. old)</t>
   </si>
   <si>
     <t>Adult</t>
   </si>
   <si>
-    <t>(18-59 yrs. old)</t>
-  </si>
-  <si>
     <t>Senior Citizens</t>
   </si>
   <si>
-    <t>(60 yrs. old and above)</t>
-  </si>
-  <si>
     <t>PWD</t>
-  </si>
-  <si>
-    <t>Pregnant Woman</t>
-  </si>
-  <si>
-    <t>Lactating Women</t>
-  </si>
-  <si>
-    <t>Evacuation Center/ Site</t>
   </si>
   <si>
     <t>Family Head</t>
@@ -143,12 +74,57 @@
   <si>
     <t>{ Barangay }</t>
   </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Pregnant 
+Woman</t>
+  </si>
+  <si>
+    <t>Lactating 
+Women</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Evacuation Center
+/ Site</t>
+  </si>
+  <si>
+    <t>Relief Services</t>
+  </si>
+  <si>
+    <t>Total No. of 
+Male</t>
+  </si>
+  <si>
+    <t>Total No. of 
+Female</t>
+  </si>
+  <si>
+    <t>Total No. of 
+Individuals</t>
+  </si>
+  <si>
+    <t>{ Age Range Here }</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +187,21 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +214,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -298,6 +305,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -305,43 +332,97 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -354,14 +435,38 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -387,7 +492,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>101463</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="657226" cy="657226"/>
     <xdr:pic>
@@ -429,15 +534,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>571501</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>472937</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>130037</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -788,236 +893,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C70A77-9BA4-454C-941D-2E52BB0F8BDA}">
-  <dimension ref="A1:N110"/>
+  <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P107" sqref="P107"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="14" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" customWidth="1"/>
+    <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-    </row>
-    <row r="5" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>22</v>
+      <c r="G8" s="31" t="s">
+        <v>24</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="H8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="15"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8" s="15"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="U9" s="12"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+    </row>
+    <row r="10" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="5" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>16</v>
+      <c r="K10" s="4" t="s">
+        <v>13</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1032,8 +1320,20 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1048,8 +1348,20 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1064,8 +1376,20 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1080,8 +1404,20 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1096,8 +1432,20 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1112,8 +1460,20 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1128,8 +1488,20 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1144,8 +1516,20 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1160,8 +1544,20 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1176,8 +1572,20 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1192,8 +1600,20 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1208,8 +1628,20 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1224,8 +1656,20 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1240,8 +1684,20 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1256,8 +1712,20 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1272,8 +1740,20 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1288,8 +1768,20 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1304,8 +1796,20 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1320,8 +1824,20 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1336,8 +1852,20 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1352,8 +1880,20 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1368,8 +1908,20 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1384,8 +1936,20 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1400,8 +1964,20 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1416,8 +1992,20 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1432,8 +2020,20 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1448,8 +2048,20 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1464,8 +2076,20 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1480,8 +2104,20 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1496,8 +2132,20 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1512,8 +2160,20 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1528,8 +2188,20 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1544,8 +2216,20 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1560,8 +2244,20 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1576,8 +2272,20 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1592,8 +2300,20 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1608,8 +2328,20 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1624,8 +2356,20 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1640,8 +2384,20 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1656,8 +2412,20 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1672,8 +2440,20 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1688,8 +2468,20 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1704,8 +2496,20 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1720,8 +2524,20 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1736,8 +2552,20 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1752,8 +2580,20 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1768,8 +2608,20 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1784,8 +2636,20 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1800,8 +2664,20 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1816,8 +2692,20 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1832,8 +2720,20 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1848,8 +2748,20 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1864,8 +2776,20 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1880,8 +2804,20 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1896,8 +2832,20 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1912,8 +2860,20 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1928,8 +2888,20 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1944,8 +2916,20 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1960,8 +2944,20 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1976,8 +2972,20 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1992,8 +3000,20 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2008,8 +3028,20 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2024,8 +3056,20 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2040,8 +3084,20 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2056,8 +3112,20 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2072,8 +3140,20 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2088,8 +3168,20 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2104,8 +3196,20 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
+      <c r="Z79" s="1"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2120,8 +3224,20 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2136,8 +3252,20 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+      <c r="Y81" s="1"/>
+      <c r="Z81" s="1"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2152,8 +3280,20 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+      <c r="Y82" s="1"/>
+      <c r="Z82" s="1"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2168,8 +3308,20 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
+      <c r="Z83" s="1"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2184,8 +3336,20 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+      <c r="Y84" s="1"/>
+      <c r="Z84" s="1"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2200,8 +3364,20 @@
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
+      <c r="Z85" s="1"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2216,8 +3392,20 @@
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2232,8 +3420,20 @@
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
+      <c r="Z87" s="1"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2248,8 +3448,20 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
+      <c r="Z88" s="1"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2264,8 +3476,20 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+      <c r="Y89" s="1"/>
+      <c r="Z89" s="1"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2280,8 +3504,20 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
+      <c r="Z90" s="1"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2296,8 +3532,20 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2312,8 +3560,20 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
+      <c r="Z92" s="1"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2328,8 +3588,20 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+      <c r="Y93" s="1"/>
+      <c r="Z93" s="1"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2344,8 +3616,20 @@
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
+      <c r="Z94" s="1"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2360,8 +3644,20 @@
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2376,8 +3672,20 @@
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+      <c r="Z96" s="1"/>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2392,8 +3700,20 @@
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+      <c r="Z97" s="1"/>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2408,8 +3728,20 @@
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
+      <c r="Z98" s="1"/>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2424,8 +3756,20 @@
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
+      <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
+      <c r="Z99" s="1"/>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2440,8 +3784,20 @@
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+      <c r="Z100" s="1"/>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2456,8 +3812,20 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2472,8 +3840,20 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+      <c r="Z102" s="1"/>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2488,8 +3868,20 @@
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+      <c r="Y103" s="1"/>
+      <c r="Z103" s="1"/>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2504,8 +3896,20 @@
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
+      <c r="Z104" s="1"/>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2520,8 +3924,20 @@
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2536,8 +3952,20 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+      <c r="T106" s="1"/>
+      <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+      <c r="Y106" s="1"/>
+      <c r="Z106" s="1"/>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2552,8 +3980,20 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="1"/>
+      <c r="S107" s="1"/>
+      <c r="T107" s="1"/>
+      <c r="U107" s="1"/>
+      <c r="V107" s="1"/>
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
+      <c r="Y107" s="1"/>
+      <c r="Z107" s="1"/>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2568,8 +4008,20 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+      <c r="T108" s="1"/>
+      <c r="U108" s="1"/>
+      <c r="V108" s="1"/>
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
+      <c r="Y108" s="1"/>
+      <c r="Z108" s="1"/>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2584,8 +4036,20 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+      <c r="Y109" s="1"/>
+      <c r="Z109" s="1"/>
+    </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2600,25 +4064,47 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+      <c r="S110" s="1"/>
+      <c r="T110" s="1"/>
+      <c r="U110" s="1"/>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+      <c r="Y110" s="1"/>
+      <c r="Z110" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:N4"/>
+  <mergeCells count="26">
+    <mergeCell ref="Z8:Z10"/>
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="A5:Z5"/>
+    <mergeCell ref="A6:Z6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A3:Z3"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="Y8:Y10"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="X8:X10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>

</xml_diff>